<commit_message>
Spelling fixes for testing file
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -61,7 +61,7 @@
     <t xml:space="preserve">Lietotājs veiksmīgi pieslēdzas izmantojot savu lietotājvārdu un e-pastu</t>
   </si>
   <si>
-    <t xml:space="preserve">Lietotājs veiksmīgi pislēdzas</t>
+    <t xml:space="preserve">Lietotājs veiksmīgi pieslēdzas</t>
   </si>
   <si>
     <t xml:space="preserve">Lietotājam ievadot veiksmīgi lietotājvārdu un neveiksmīgi e-pastu tiek prasīta atkārtota pieslēgšanās</t>
@@ -79,7 +79,7 @@
     <t xml:space="preserve">Veiksmīgi izvada visas grāmatas ar to laukiem (ID, nosaukums, autors, izdošanas gads, žanrs un cena)</t>
   </si>
   <si>
-    <t xml:space="preserve">Izvada lietotāja lasāmso sarakstu ar tā laukiem (ID, nosaukums, autors, izdošanas gads,žanrs, cena un tās status – izlasīta vai neizlasīta)</t>
+    <t xml:space="preserve">Izvada lietotāja lasāmo sarakstu ar tā laukiem (ID, nosaukums, autors, izdošanas gads,žanrs, cena un tās status – izlasīta vai neizlasīta)</t>
   </si>
   <si>
     <t xml:space="preserve">Veiksmīgi izvada sarakstu ar tā laukiem (ID, nosaukums, autors, izdošanas gads, žanrs, cena un status)</t>
@@ -88,7 +88,7 @@
     <t xml:space="preserve">Grāmatu kārtošana</t>
   </si>
   <si>
-    <t xml:space="preserve">Iespējams kārtot grāmatas pēc nosaukuma, autora, cenas, gada vai id (visus iespējams kārtot augstošā vai dilstošā secībā)</t>
+    <t xml:space="preserve">Iespējams kārtot grāmatas pēc nosaukuma, autora, cenas, gada vai id (visus iespējams kārtot augošā vai dilstošā secībā)</t>
   </si>
   <si>
     <t xml:space="preserve">Grāmatas tiek sakārtotas pēc prasībām</t>
@@ -139,7 +139,7 @@
     <t xml:space="preserve">Ievadot grāmatas id, grāmata tiek pievienota pie lietotāja lasāmā saraksta</t>
   </si>
   <si>
-    <t xml:space="preserve">Lietotājs ievada id un tiek dota ziņa, ka attiecošā grāmata jau ir pievienota</t>
+    <t xml:space="preserve">Lietotājs ievada id un tiek dota ziņa, ka izvēlētā grāmata jau ir pievienota</t>
   </si>
   <si>
     <t xml:space="preserve">Ievadot grāmatas id, dod ziņu, ka tā jau ir pievienota</t>
@@ -196,6 +196,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -217,6 +218,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -268,32 +270,36 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -423,289 +429,289 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="29.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="35.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="33.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="29.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="26.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="23.79"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="58.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
+      <c r="A2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="4"/>
+      <c r="H2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="68.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
+      <c r="A3" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="64.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
+      <c r="A4" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
+      <c r="A5" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="55.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
+      <c r="A6" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="68.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
+      <c r="A7" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="70.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
+      <c r="A8" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="73.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
+      <c r="A9" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="66.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="n">
+      <c r="A10" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="66.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="n">
+      <c r="A11" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="64.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>